<commit_message>
Updated VT Phone Number population logic
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/VT-Data.xlsx
+++ b/KatalonData/Bootstrap/VT-Data.xlsx
@@ -1,47 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{494AB31C-6A44-4BBC-B202-6EB7FC619A0D}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00E9DD3-FC41-43D0-B3CA-9989048819B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="24" firstSheet="22" tabRatio="771" windowHeight="12990" windowWidth="13230" xWindow="32580" xr2:uid="{F6D5B6E5-5530-44B1-A3FD-270D512FE765}" yWindow="1830"/>
+    <workbookView xWindow="2355" yWindow="3075" windowWidth="25710" windowHeight="10710" tabRatio="771" firstSheet="20" activeTab="20" xr2:uid="{F6D5B6E5-5530-44B1-A3FD-270D512FE765}"/>
   </bookViews>
   <sheets>
-    <sheet name="VT-Sale-NoCF" r:id="rId1" sheetId="1"/>
-    <sheet name="VT-Auth-NoCF" r:id="rId2" sheetId="2"/>
-    <sheet name="VT-SaleVoid-NoCF" r:id="rId3" sheetId="3"/>
-    <sheet name="VT-Sale-NoCF-QA" r:id="rId4" sheetId="6"/>
-    <sheet name="VT-Sale-NoCF-Demo" r:id="rId5" sheetId="4"/>
-    <sheet name="VT-Sale-NoCF-Prod" r:id="rId6" sheetId="5"/>
-    <sheet name="VT-Sale-NoCF-Generic" r:id="rId7" sheetId="9"/>
-    <sheet name="VT-Sale-SingleCF-Generic" r:id="rId8" sheetId="10"/>
-    <sheet name="VT-Sale-DualCF-Generic" r:id="rId9" sheetId="11"/>
-    <sheet name="VT-Auth-NoCF-Generic" r:id="rId10" sheetId="12"/>
-    <sheet name="VT-Auth-SingleCF-Generic" r:id="rId11" sheetId="13"/>
-    <sheet name="VT-Auth-DualCF-Generic" r:id="rId12" sheetId="14"/>
-    <sheet name="VT-SaleVoid-NoCF-Generic" r:id="rId13" sheetId="15"/>
-    <sheet name="VT-SaleVoid-SingleCF-Generic" r:id="rId14" sheetId="16"/>
-    <sheet name="VT-SaleVoid-DualCF-Generic" r:id="rId15" sheetId="17"/>
-    <sheet name="VT-SaleCredit-NoCF-Generic" r:id="rId16" sheetId="18"/>
-    <sheet name="VT-SaleCredit-SingleCF-Generic" r:id="rId17" sheetId="19"/>
-    <sheet name="VT-SaleCredit-DualCF-Generic" r:id="rId18" sheetId="20"/>
-    <sheet name="VT-AuthCapture-NoCF-Generic" r:id="rId19" sheetId="21"/>
-    <sheet name="VT-AuthCapture-SingleCF-Generic" r:id="rId20" sheetId="22"/>
-    <sheet name="VT-AuthCapture-DualCF-Generic" r:id="rId21" sheetId="23"/>
-    <sheet name="VT-ManualAuthCapture-Generic" r:id="rId22" sheetId="24"/>
-    <sheet name="VT-AuthCapVoid-Generic" r:id="rId23" sheetId="25"/>
-    <sheet name="VT-AuthCapCredit-Generic" r:id="rId24" sheetId="26"/>
-    <sheet name="VT-Sale-CC" r:id="rId25" sheetId="27"/>
+    <sheet name="VT-Sale-NoCF" sheetId="1" r:id="rId1"/>
+    <sheet name="VT-Auth-NoCF" sheetId="2" r:id="rId2"/>
+    <sheet name="VT-SaleVoid-NoCF" sheetId="3" r:id="rId3"/>
+    <sheet name="VT-Sale-NoCF-QA" sheetId="6" r:id="rId4"/>
+    <sheet name="VT-Sale-NoCF-Demo" sheetId="4" r:id="rId5"/>
+    <sheet name="VT-Sale-NoCF-Prod" sheetId="5" r:id="rId6"/>
+    <sheet name="VT-Sale-NoCF-Generic" sheetId="9" r:id="rId7"/>
+    <sheet name="VT-Sale-SingleCF-Generic" sheetId="10" r:id="rId8"/>
+    <sheet name="VT-Sale-DualCF-Generic" sheetId="11" r:id="rId9"/>
+    <sheet name="VT-Auth-NoCF-Generic" sheetId="12" r:id="rId10"/>
+    <sheet name="VT-Auth-SingleCF-Generic" sheetId="13" r:id="rId11"/>
+    <sheet name="VT-Auth-DualCF-Generic" sheetId="14" r:id="rId12"/>
+    <sheet name="VT-SaleVoid-NoCF-Generic" sheetId="15" r:id="rId13"/>
+    <sheet name="VT-SaleVoid-SingleCF-Generic" sheetId="16" r:id="rId14"/>
+    <sheet name="VT-SaleVoid-DualCF-Generic" sheetId="17" r:id="rId15"/>
+    <sheet name="VT-SaleCredit-NoCF-Generic" sheetId="18" r:id="rId16"/>
+    <sheet name="VT-SaleCredit-SingleCF-Generic" sheetId="19" r:id="rId17"/>
+    <sheet name="VT-SaleCredit-DualCF-Generic" sheetId="20" r:id="rId18"/>
+    <sheet name="VT-AuthCapture-NoCF-Generic" sheetId="21" r:id="rId19"/>
+    <sheet name="VT-AuthCapture-SingleCF-Generic" sheetId="22" r:id="rId20"/>
+    <sheet name="VT-AuthCapture-DualCF-Generic" sheetId="23" r:id="rId21"/>
+    <sheet name="VT-ManualAuthCapture-Generic" sheetId="24" r:id="rId22"/>
+    <sheet name="VT-AuthCapVoid-Generic" sheetId="25" r:id="rId23"/>
+    <sheet name="VT-AuthCapCredit-Generic" sheetId="26" r:id="rId24"/>
+    <sheet name="VT-Sale-CC" sheetId="27" r:id="rId25"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6286" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6278" uniqueCount="112">
   <si>
     <t>Result</t>
   </si>
@@ -394,15 +394,6 @@
     <t>Pass</t>
   </si>
   <si>
-    <t>Sat Jul 20 17:25:24 EDT 2024</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Sat Jul 20 17:43:54 EDT 2024</t>
-  </si>
-  <si>
     <t>Sat Jul 20 17:45:07 EDT 2024</t>
   </si>
 </sst>
@@ -410,7 +401,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -459,19 +449,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -488,10 +478,10 @@
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -526,7 +516,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -578,7 +568,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -689,21 +679,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -720,7 +710,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -772,35 +762,35 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office 2013 - 2022 Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91B27BFE-C179-457F-B2B0-1744259BA9C2}">
-  <dimension ref="A1:AF9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91B27BFE-C179-457F-B2B0-1744259BA9C2}">
+  <dimension ref="A1:AE9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" style="1" width="12.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="6.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="20.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="22.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="30.5703125" collapsed="true"/>
-    <col min="10" max="12" style="1" width="12.140625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="1" width="24.42578125" collapsed="true"/>
-    <col min="14" max="28" style="1" width="12.140625" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" style="1" width="20.42578125" collapsed="true"/>
-    <col min="30" max="30" style="1" width="12.140625" collapsed="true"/>
-    <col min="31" max="31" customWidth="true" style="1" width="24.7109375" collapsed="true"/>
-    <col min="32" max="16384" style="1" width="12.140625" collapsed="true"/>
+    <col min="1" max="4" width="12.140625" style="1" collapsed="1"/>
+    <col min="5" max="5" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="30.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="12" width="12.140625" style="1" collapsed="1"/>
+    <col min="13" max="13" width="24.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="28" width="12.140625" style="1" collapsed="1"/>
+    <col min="29" max="29" width="20.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12.140625" style="1" collapsed="1"/>
+    <col min="31" max="31" width="24.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="16384" width="12.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
@@ -1540,8 +1530,8 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1549,51 +1539,51 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B46B067-4265-4DD4-9E53-9D7B3D6A04D6}">
-  <dimension ref="A1:AJ9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B46B067-4265-4DD4-9E53-9D7B3D6A04D6}">
+  <dimension ref="A1:AI9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="J17" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="22.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="28.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="32.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="4.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="7.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="17.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="5.85546875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="13.7109375" collapsed="true"/>
-    <col min="36" max="16384" style="1" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="28.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="32.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="16384" width="12.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
@@ -2440,7 +2430,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -2448,51 +2438,51 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06261D80-2EB2-47BF-A617-689143884D3A}">
-  <dimension ref="A1:AJ9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06261D80-2EB2-47BF-A617-689143884D3A}">
+  <dimension ref="A1:AI9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="27.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="32.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="34.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="4.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="7.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="17.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="5.85546875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="13.7109375" collapsed="true"/>
-    <col min="36" max="16384" style="1" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="32.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="34.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="16384" width="12.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
@@ -3339,7 +3329,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3347,51 +3337,51 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5194EEE-324C-4DC0-9E8A-39144144E59B}">
-  <dimension ref="A1:AJ9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5194EEE-324C-4DC0-9E8A-39144144E59B}">
+  <dimension ref="A1:AI9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="27.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="32.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="34.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="4.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="7.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="17.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="5.85546875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="13.7109375" collapsed="true"/>
-    <col min="36" max="16384" style="1" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="32.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="34.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="16384" width="12.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
@@ -4238,7 +4228,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -4246,51 +4236,51 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{241DB443-37F6-4A04-B2C1-F3B4B2D449F4}">
-  <dimension ref="A1:AJ9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{241DB443-37F6-4A04-B2C1-F3B4B2D449F4}">
+  <dimension ref="A1:AI9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="22.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="28.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="32.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="4.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="7.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="17.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="5.85546875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="13.7109375" collapsed="true"/>
-    <col min="36" max="16384" style="1" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="28.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="32.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="16384" width="12.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
@@ -5137,7 +5127,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -5145,51 +5135,51 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DF30BA6-87C6-4620-8EBD-E4C32AC519D9}">
-  <dimension ref="A1:AJ9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DF30BA6-87C6-4620-8EBD-E4C32AC519D9}">
+  <dimension ref="A1:AI9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="27.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="32.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="34.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="4.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="7.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="17.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="5.85546875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="13.7109375" collapsed="true"/>
-    <col min="36" max="16384" style="1" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="32.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="34.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="16384" width="12.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
@@ -6036,7 +6026,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -6044,51 +6034,51 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6204D91-76F9-4D6D-A5E4-EB5CFE343B83}">
-  <dimension ref="A1:AJ9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6204D91-76F9-4D6D-A5E4-EB5CFE343B83}">
+  <dimension ref="A1:AI9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="27.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="32.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="34.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="4.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="7.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="17.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="5.85546875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="13.7109375" collapsed="true"/>
-    <col min="36" max="16384" style="1" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="32.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="34.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="16384" width="12.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
@@ -6935,7 +6925,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -6943,51 +6933,51 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6BF78E2-2FD7-4E12-B170-A75AAE6742DA}">
-  <dimension ref="A1:AJ9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6BF78E2-2FD7-4E12-B170-A75AAE6742DA}">
+  <dimension ref="A1:AI9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="22.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="28.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="32.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="4.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="7.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="17.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="5.85546875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="13.7109375" collapsed="true"/>
-    <col min="36" max="16384" style="1" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="28.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="32.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="16384" width="12.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
@@ -7834,7 +7824,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -7842,52 +7832,52 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B03DBA54-ED01-4791-84D7-55AE2E626F53}">
-  <dimension ref="A1:AK9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B03DBA54-ED01-4791-84D7-55AE2E626F53}">
+  <dimension ref="A1:AJ9"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="AI13" sqref="AI13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="27.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="32.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="34.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="4.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="7.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="17.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="5.85546875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="13.7109375" collapsed="true"/>
-    <col min="36" max="36" customWidth="true" style="1" width="21.5703125" collapsed="true"/>
-    <col min="37" max="16384" style="1" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="32.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="34.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="21.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="16384" width="12.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
@@ -8761,7 +8751,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -8769,51 +8759,51 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB20E3F1-C4A0-4DB3-BD74-0C25E6E1CBA8}">
-  <dimension ref="A1:AJ9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB20E3F1-C4A0-4DB3-BD74-0C25E6E1CBA8}">
+  <dimension ref="A1:AI9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="27.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="32.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="34.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="4.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="7.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="17.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="5.85546875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="13.7109375" collapsed="true"/>
-    <col min="36" max="16384" style="1" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="32.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="34.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="16384" width="12.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
@@ -9660,7 +9650,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -9668,52 +9658,52 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E27B5D9-5032-44E3-84E3-DE165915798B}">
-  <dimension ref="A1:AK9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E27B5D9-5032-44E3-84E3-DE165915798B}">
+  <dimension ref="A1:AJ9"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
+    <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="AJ1" sqref="AJ1:AJ9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="22.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="28.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="32.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="4.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="7.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="17.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="5.85546875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="13.7109375" collapsed="true"/>
-    <col min="36" max="36" customWidth="true" style="1" width="18.42578125" collapsed="true"/>
-    <col min="37" max="16384" style="1" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="28.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="32.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="18.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="16384" width="12.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
@@ -10587,7 +10577,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -10595,28 +10585,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F1476F1-7EFE-4E48-BC46-8549E9104F90}">
-  <dimension ref="A1:AF9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F1476F1-7EFE-4E48-BC46-8549E9104F90}">
+  <dimension ref="A1:AE9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" style="1" width="12.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="6.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="20.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="22.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="30.5703125" collapsed="true"/>
-    <col min="10" max="12" style="1" width="12.140625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="1" width="24.42578125" collapsed="true"/>
-    <col min="14" max="28" style="1" width="12.140625" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" style="1" width="20.42578125" collapsed="true"/>
-    <col min="30" max="30" style="1" width="12.140625" collapsed="true"/>
-    <col min="31" max="31" customWidth="true" style="1" width="24.7109375" collapsed="true"/>
-    <col min="32" max="16384" style="1" width="12.140625" collapsed="true"/>
+    <col min="1" max="4" width="12.140625" style="1" collapsed="1"/>
+    <col min="5" max="5" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="30.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="12" width="12.140625" style="1" collapsed="1"/>
+    <col min="13" max="13" width="24.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="28" width="12.140625" style="1" collapsed="1"/>
+    <col min="29" max="29" width="20.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12.140625" style="1" collapsed="1"/>
+    <col min="31" max="31" width="24.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="16384" width="12.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
@@ -11355,7 +11345,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -11363,8 +11353,8 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{032979C1-8E13-45E8-AA46-AA2C52C9A8C1}">
-  <dimension ref="A1:AL9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{032979C1-8E13-45E8-AA46-AA2C52C9A8C1}">
+  <dimension ref="A1:AK9"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="AK1" sqref="AK1:AK9"/>
@@ -11372,44 +11362,44 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="27.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="32.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="34.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="4.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="7.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="17.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="5.85546875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="13.7109375" collapsed="true"/>
-    <col min="36" max="36" customWidth="true" style="1" width="19.140625" collapsed="true"/>
-    <col min="37" max="37" customWidth="true" style="1" width="18.7109375" collapsed="true"/>
-    <col min="38" max="16384" style="1" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="32.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="34.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="19.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="18.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="16384" width="12.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -12310,7 +12300,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -12318,53 +12308,53 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C1337E-1CCF-48A2-B6FB-BAE32E7E4A51}">
-  <dimension ref="A1:AL9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C1337E-1CCF-48A2-B6FB-BAE32E7E4A51}">
+  <dimension ref="A1:AK9"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
       <selection activeCell="AK1" sqref="AK1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="27.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="32.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="34.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="4.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="7.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="17.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="5.85546875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="13.7109375" collapsed="true"/>
-    <col min="36" max="36" customWidth="true" style="1" width="16.85546875" collapsed="true"/>
-    <col min="37" max="37" customWidth="true" style="1" width="18.5703125" collapsed="true"/>
-    <col min="38" max="16384" style="1" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="32.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="34.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="16.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="18.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="16384" width="12.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -13265,7 +13255,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -13273,55 +13263,55 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17271EBE-670B-4D28-BBDF-B37E570C7236}">
-  <dimension ref="A1:AK7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17271EBE-670B-4D28-BBDF-B37E570C7236}">
+  <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.140625" defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="31.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="28.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="32.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="4.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="7.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="17.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="5.85546875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="13.7109375" collapsed="true"/>
-    <col min="36" max="36" customWidth="true" style="1" width="18.42578125" collapsed="true"/>
-    <col min="37" max="16384" style="1" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="31.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="28.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="32.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="18.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="16384" width="12.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="15" r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -13431,7 +13421,7 @@
         <v>99</v>
       </c>
     </row>
-    <row ht="15" r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="D2" s="1" t="s">
         <v>67</v>
       </c>
@@ -13526,7 +13516,7 @@
         <v>36</v>
       </c>
     </row>
-    <row ht="15" r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
         <v>67</v>
       </c>
@@ -13621,7 +13611,7 @@
         <v>100</v>
       </c>
     </row>
-    <row ht="30" r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" ht="30" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
         <v>67</v>
       </c>
@@ -13716,7 +13706,7 @@
         <v>36</v>
       </c>
     </row>
-    <row ht="30" r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" ht="30" x14ac:dyDescent="0.25">
       <c r="D5" s="1" t="s">
         <v>67</v>
       </c>
@@ -13811,7 +13801,7 @@
         <v>100</v>
       </c>
     </row>
-    <row ht="15" r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
         <v>67</v>
       </c>
@@ -13906,7 +13896,7 @@
         <v>36</v>
       </c>
     </row>
-    <row ht="15" r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
         <v>67</v>
       </c>
@@ -14002,7 +13992,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -14010,55 +14000,55 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62AD5C19-1571-4D0A-A553-7E96DEC1AB05}">
-  <dimension ref="A1:AK7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62AD5C19-1571-4D0A-A553-7E96DEC1AB05}">
+  <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.140625" defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="31.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="28.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="32.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="4.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="7.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="17.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="5.85546875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="13.7109375" collapsed="true"/>
-    <col min="36" max="36" customWidth="true" style="1" width="18.42578125" collapsed="true"/>
-    <col min="37" max="16384" style="1" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="31.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="28.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="32.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="18.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="16384" width="12.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="15" r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -14168,7 +14158,7 @@
         <v>99</v>
       </c>
     </row>
-    <row ht="15" r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="D2" s="1" t="s">
         <v>67</v>
       </c>
@@ -14263,7 +14253,7 @@
         <v>36</v>
       </c>
     </row>
-    <row ht="15" r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
         <v>67</v>
       </c>
@@ -14358,7 +14348,7 @@
         <v>100</v>
       </c>
     </row>
-    <row ht="30" r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" ht="30" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
         <v>67</v>
       </c>
@@ -14453,7 +14443,7 @@
         <v>36</v>
       </c>
     </row>
-    <row ht="30" r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" ht="30" x14ac:dyDescent="0.25">
       <c r="D5" s="1" t="s">
         <v>67</v>
       </c>
@@ -14548,7 +14538,7 @@
         <v>100</v>
       </c>
     </row>
-    <row ht="15" r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
         <v>67</v>
       </c>
@@ -14643,7 +14633,7 @@
         <v>36</v>
       </c>
     </row>
-    <row ht="15" r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
         <v>67</v>
       </c>
@@ -14739,7 +14729,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -14747,55 +14737,55 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9831DEED-0542-40B2-842B-1196FAE6B383}">
-  <dimension ref="A1:AK5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9831DEED-0542-40B2-842B-1196FAE6B383}">
+  <dimension ref="A1:AJ5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.140625" defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="9.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="26.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="33.5703125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="27.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="4.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="7.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="17.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="5.85546875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="13.7109375" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" style="1" width="15.28515625" collapsed="true"/>
-    <col min="37" max="16384" style="1" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="26.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="33.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="27.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="15.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="16384" width="12.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="15" r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -14905,7 +14895,7 @@
         <v>99</v>
       </c>
     </row>
-    <row ht="15" r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="D2" s="1" t="s">
         <v>67</v>
       </c>
@@ -15000,7 +14990,7 @@
         <v>36</v>
       </c>
     </row>
-    <row ht="15" r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
         <v>67</v>
       </c>
@@ -15095,7 +15085,7 @@
         <v>100</v>
       </c>
     </row>
-    <row ht="15" r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
         <v>67</v>
       </c>
@@ -15190,7 +15180,7 @@
         <v>36</v>
       </c>
     </row>
-    <row ht="15" r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="D5" s="1" t="s">
         <v>67</v>
       </c>
@@ -15286,7 +15276,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -15294,30 +15284,30 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15EA71D8-85A1-4E2F-99AC-6F1992B650B9}">
-  <dimension ref="A1:AG2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15EA71D8-85A1-4E2F-99AC-6F1992B650B9}">
+  <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="AG2" sqref="AG2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.140625" collapsed="true"/>
-    <col min="3" max="4" style="1" width="12.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="6.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="20.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="22.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="30.5703125" collapsed="true"/>
-    <col min="10" max="12" style="1" width="12.140625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="1" width="24.42578125" collapsed="true"/>
-    <col min="14" max="28" style="1" width="12.140625" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" style="1" width="20.42578125" collapsed="true"/>
-    <col min="30" max="30" style="1" width="12.140625" collapsed="true"/>
-    <col min="31" max="32" customWidth="true" style="1" width="24.7109375" collapsed="true"/>
-    <col min="33" max="16384" style="1" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="25.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="12.140625" style="1" collapsed="1"/>
+    <col min="5" max="5" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="30.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="12" width="12.140625" style="1" collapsed="1"/>
+    <col min="13" max="13" width="24.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="28" width="12.140625" style="1" collapsed="1"/>
+    <col min="29" max="29" width="20.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12.140625" style="1" collapsed="1"/>
+    <col min="31" max="32" width="24.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="16384" width="12.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
@@ -15423,7 +15413,7 @@
         <v>110</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>67</v>
@@ -15508,33 +15498,33 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6327E26-4C79-4401-A8C5-21FF97F5A24E}">
-  <dimension ref="A1:AF9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6327E26-4C79-4401-A8C5-21FF97F5A24E}">
+  <dimension ref="A1:AE9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" style="1" width="12.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="6.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="20.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="22.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="30.5703125" collapsed="true"/>
-    <col min="10" max="12" style="1" width="12.140625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="1" width="24.42578125" collapsed="true"/>
-    <col min="14" max="28" style="1" width="12.140625" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" style="1" width="20.42578125" collapsed="true"/>
-    <col min="30" max="30" style="1" width="12.140625" collapsed="true"/>
-    <col min="31" max="31" customWidth="true" style="1" width="24.7109375" collapsed="true"/>
-    <col min="32" max="16384" style="1" width="12.140625" collapsed="true"/>
+    <col min="1" max="4" width="12.140625" style="1" collapsed="1"/>
+    <col min="5" max="5" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="30.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="12" width="12.140625" style="1" collapsed="1"/>
+    <col min="13" max="13" width="24.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="28" width="12.140625" style="1" collapsed="1"/>
+    <col min="29" max="29" width="20.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12.140625" style="1" collapsed="1"/>
+    <col min="31" max="31" width="24.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="16384" width="12.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
@@ -16273,7 +16263,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -16281,28 +16271,28 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29E4099-67A8-4B75-B256-0F3E875A0236}">
-  <dimension ref="A1:AF9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29E4099-67A8-4B75-B256-0F3E875A0236}">
+  <dimension ref="A1:AE9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" style="1" width="12.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="6.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="20.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="22.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="30.5703125" collapsed="true"/>
-    <col min="10" max="12" style="1" width="12.140625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="1" width="24.42578125" collapsed="true"/>
-    <col min="14" max="28" style="1" width="12.140625" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" style="1" width="20.42578125" collapsed="true"/>
-    <col min="30" max="30" style="1" width="12.140625" collapsed="true"/>
-    <col min="31" max="31" customWidth="true" style="1" width="24.7109375" collapsed="true"/>
-    <col min="32" max="16384" style="1" width="12.140625" collapsed="true"/>
+    <col min="1" max="4" width="12.140625" style="1" collapsed="1"/>
+    <col min="5" max="5" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="30.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="12" width="12.140625" style="1" collapsed="1"/>
+    <col min="13" max="13" width="24.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="28" width="12.140625" style="1" collapsed="1"/>
+    <col min="29" max="29" width="20.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12.140625" style="1" collapsed="1"/>
+    <col min="31" max="31" width="24.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="16384" width="12.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
@@ -17041,7 +17031,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -17049,28 +17039,28 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20F0B3AF-1323-47BA-A321-CEBD9FBB27E2}">
-  <dimension ref="A1:AF9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20F0B3AF-1323-47BA-A321-CEBD9FBB27E2}">
+  <dimension ref="A1:AE9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" style="1" width="12.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="6.42578125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="33.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="22.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="30.5703125" collapsed="true"/>
-    <col min="10" max="12" style="1" width="12.140625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="1" width="24.42578125" collapsed="true"/>
-    <col min="14" max="28" style="1" width="12.140625" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" style="1" width="20.42578125" collapsed="true"/>
-    <col min="30" max="30" style="1" width="12.140625" collapsed="true"/>
-    <col min="31" max="31" customWidth="true" style="1" width="24.7109375" collapsed="true"/>
-    <col min="32" max="16384" style="1" width="12.140625" collapsed="true"/>
+    <col min="1" max="4" width="12.140625" style="1" collapsed="1"/>
+    <col min="5" max="5" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="33.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="30.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="12" width="12.140625" style="1" collapsed="1"/>
+    <col min="13" max="13" width="24.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="28" width="12.140625" style="1" collapsed="1"/>
+    <col min="29" max="29" width="20.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12.140625" style="1" collapsed="1"/>
+    <col min="31" max="31" width="24.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="16384" width="12.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
@@ -17809,8 +17799,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -17818,28 +17808,28 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19FEF63A-9B81-4958-ACAF-2A5DC6F5B6C0}">
-  <dimension ref="A1:AF9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19FEF63A-9B81-4958-ACAF-2A5DC6F5B6C0}">
+  <dimension ref="A1:AE9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" style="1" width="12.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="6.42578125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="36.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="22.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="30.5703125" collapsed="true"/>
-    <col min="10" max="12" style="1" width="12.140625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="1" width="24.42578125" collapsed="true"/>
-    <col min="14" max="28" style="1" width="12.140625" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" style="1" width="20.42578125" collapsed="true"/>
-    <col min="30" max="30" style="1" width="12.140625" collapsed="true"/>
-    <col min="31" max="31" customWidth="true" style="1" width="24.7109375" collapsed="true"/>
-    <col min="32" max="16384" style="1" width="12.140625" collapsed="true"/>
+    <col min="1" max="4" width="12.140625" style="1" collapsed="1"/>
+    <col min="5" max="5" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="36.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="30.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="12" width="12.140625" style="1" collapsed="1"/>
+    <col min="13" max="13" width="24.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="28" width="12.140625" style="1" collapsed="1"/>
+    <col min="29" max="29" width="20.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12.140625" style="1" collapsed="1"/>
+    <col min="31" max="31" width="24.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="16384" width="12.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
@@ -18578,7 +18568,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -18586,51 +18576,51 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F87D544-043A-4E2A-88AC-E2072E1F830C}">
-  <dimension ref="A1:AJ9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F87D544-043A-4E2A-88AC-E2072E1F830C}">
+  <dimension ref="A1:AI9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="22.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="28.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="32.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="4.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="7.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="17.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="5.85546875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="13.7109375" collapsed="true"/>
-    <col min="36" max="16384" style="1" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="28.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="32.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="16384" width="12.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
@@ -19477,7 +19467,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -19485,51 +19475,51 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B968B157-8910-471B-87BA-7CC46E0AB45F}">
-  <dimension ref="A1:AJ9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B968B157-8910-471B-87BA-7CC46E0AB45F}">
+  <dimension ref="A1:AI9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="27.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="32.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="34.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="4.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="7.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="17.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="5.85546875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="13.7109375" collapsed="true"/>
-    <col min="36" max="16384" style="1" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="32.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="34.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="16384" width="12.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
@@ -20376,7 +20366,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -20384,51 +20374,51 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69067CF8-28FC-4E68-B131-0C0578E97988}">
-  <dimension ref="A1:AJ9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69067CF8-28FC-4E68-B131-0C0578E97988}">
+  <dimension ref="A1:AI9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="27.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="32.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="34.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="4.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="7.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="17.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="5.85546875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="13.7109375" collapsed="true"/>
-    <col min="36" max="16384" style="1" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="32.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="34.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="16384" width="12.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
@@ -21275,7 +21265,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>

</xml_diff>